<commit_message>
distance: Implement Cosine distance
</commit_message>
<xml_diff>
--- a/Orange/distance/tests/calculation.xlsx
+++ b/Orange/distance/tests/calculation.xlsx
@@ -9,17 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="10"/>
   </bookViews>
   <sheets>
-    <sheet name="disc" sheetId="2" r:id="rId1"/>
+    <sheet name="disc - eucl+manh" sheetId="2" r:id="rId1"/>
     <sheet name="cont - eucl" sheetId="1" r:id="rId2"/>
     <sheet name="mixed - eucl" sheetId="3" r:id="rId3"/>
     <sheet name="two-tables - eucl" sheetId="4" r:id="rId4"/>
     <sheet name="cont - manh" sheetId="5" r:id="rId5"/>
     <sheet name="mixed - manh" sheetId="6" r:id="rId6"/>
     <sheet name="two-tables - manh" sheetId="7" r:id="rId7"/>
-    <sheet name="jaccard" sheetId="8" r:id="rId8"/>
+    <sheet name="cont - cosine" sheetId="9" r:id="rId8"/>
+    <sheet name="disc - cosine" sheetId="10" r:id="rId9"/>
+    <sheet name="mixed - cosine" sheetId="11" r:id="rId10"/>
+    <sheet name="two-tables - cosine" sheetId="12" r:id="rId11"/>
+    <sheet name="jaccard" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>BY ROWS - NORMALIZED</t>
   </si>
@@ -70,6 +74,15 @@
   </si>
   <si>
     <t>bc</t>
+  </si>
+  <si>
+    <t>BY ROWS</t>
+  </si>
+  <si>
+    <t>BY COLUMNS</t>
+  </si>
+  <si>
+    <t>abs</t>
   </si>
 </sst>
 </file>
@@ -155,7 +168,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -263,8 +276,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -281,8 +310,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -336,6 +368,14 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -389,6 +429,14 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -805,12 +853,1220 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:T7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>SQRT(15)</f>
+        <v>3.872983346207417</v>
+      </c>
+      <c r="I3">
+        <f>A3*A4</f>
+        <v>-1</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="0">B3*B4</f>
+        <v>15</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K5" si="1">C3*C4</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>SUM(I3:K3)</f>
+        <v>14</v>
+      </c>
+      <c r="M3">
+        <f>L3</f>
+        <v>14</v>
+      </c>
+      <c r="N3">
+        <f>M3/G3/G4</f>
+        <v>0.68313005106397318</v>
+      </c>
+      <c r="O3">
+        <f>1-COS(N3)</f>
+        <v>0.22439924133143663</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>O3</f>
+        <v>0.22439924133143663</v>
+      </c>
+      <c r="T3">
+        <f>O5</f>
+        <v>0.30926431717875691</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-1</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f>SQRT(28)</f>
+        <v>5.2915026221291814</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I5" si="2">A4*A5</f>
+        <v>-1</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L5" si="3">SUM(I4:K4)</f>
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <f>L4+1</f>
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <f>M4/G4/G5</f>
+        <v>0.42257712736425829</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O5" si="4">1-COS(N4)</f>
+        <v>8.796494132354804E-2</v>
+      </c>
+      <c r="R4">
+        <f>O3</f>
+        <v>0.22439924133143663</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f>O4</f>
+        <v>8.796494132354804E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>SQRT(5)</f>
+        <v>2.2360679774997898</v>
+      </c>
+      <c r="I5">
+        <f>A3*A5</f>
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:K5" si="5">B3*B5</f>
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <f>L5+1</f>
+        <v>7</v>
+      </c>
+      <c r="N5">
+        <f>M5/G3/G5</f>
+        <v>0.808290376865476</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>0.30926431717875691</v>
+      </c>
+      <c r="R5">
+        <f>O5</f>
+        <v>0.30926431717875691</v>
+      </c>
+      <c r="S5">
+        <f>O4</f>
+        <v>8.796494132354804E-2</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f>AVERAGE(A3:A5)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:C6" si="6">AVERAGE(B3:B5)</f>
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E6" s="4">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F6" s="4">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>_xlfn.VAR.P(A3:A5)</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ref="B7:C7" si="7">_xlfn.VAR.P(B3:B5)</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="7"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7">
+        <v>-1</v>
+      </c>
+      <c r="E7">
+        <v>-1</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:N30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f>A3^2</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:G6" si="0">B3^2</f>
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <f>SQRT(SUM(E3:G3))</f>
+        <v>3.7416573867739413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>A7^2 + A8</f>
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="1">SQRT(SUM(E4:G4))</f>
+        <v>6.4807406984078604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E7" si="2">A5^2</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.7320508075688772</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>7.8740078740118111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>AVERAGE(A3:A6)</f>
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ref="B7:C7" si="3">AVERAGE(B3:B6)</f>
+        <v>2.75</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f>_xlfn.VAR.P(A3:A6)</f>
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ref="B8:C8" si="4">_xlfn.VAR.P(B3:B6)</f>
+        <v>2.1875</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f>A22^2</f>
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:F23" si="5">B22^2</f>
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G23" si="6">C22^2</f>
+        <v>9</v>
+      </c>
+      <c r="H22">
+        <f>SQRT(SUM(E22:G22))</f>
+        <v>3.7416573867739413</v>
+      </c>
+      <c r="J22">
+        <f>A$22*A3</f>
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ref="K22:L22" si="7">B$22*B3</f>
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="M22">
+        <f>SUM(J22:L22)</f>
+        <v>11</v>
+      </c>
+      <c r="N22">
+        <f>1-COS(M22)</f>
+        <v>0.99557430201194919</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <f>A7^2 + A8</f>
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23" si="8">SQRT(SUM(E23:G23))</f>
+        <v>5</v>
+      </c>
+      <c r="J23">
+        <f>A7*A4</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="J23:L23" si="9">B$22*B4</f>
+        <v>5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:M25" si="10">SUM(J23:L23)</f>
+        <v>5</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ref="N23:N30" si="11">1-COS(M23)</f>
+        <v>0.71633781453677381</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <f t="shared" ref="J24:L24" si="12">A$22*A5</f>
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="11"/>
+        <v>3.9829713349634033E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <f t="shared" ref="J25:L25" si="13">A$22*A6</f>
+        <v>14</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="13"/>
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="11"/>
+        <v>8.7971881365264126E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <f>A$7*A3</f>
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ref="K27:L27" si="14">B$23*B3</f>
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ref="M27:M30" si="15">SUM(J27:L27)</f>
+        <v>13</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="11"/>
+        <v>9.2553218549803806E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <f>A$7^2</f>
+        <v>9</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ref="J28:L28" si="16">B$23*B4</f>
+        <v>10</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="15"/>
+        <v>19</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="11"/>
+        <v>1.1295381813330785E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <f t="shared" ref="J28:J30" si="17">A$7*A5</f>
+        <v>3</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="J29:L29" si="18">B$23*B5</f>
+        <v>2</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="11"/>
+        <v>0.2460977456566954</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <f t="shared" si="17"/>
+        <v>21</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ref="J30:L30" si="19">B$23*B6</f>
+        <v>4</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="19"/>
+        <v>6</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="15"/>
+        <v>31</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="11"/>
+        <v>8.5257642195468719E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1">
+        <v>12</v>
+      </c>
+      <c r="F1">
+        <v>13</v>
+      </c>
+      <c r="G1">
+        <v>14</v>
+      </c>
+      <c r="H1">
+        <v>23</v>
+      </c>
+      <c r="I1">
+        <v>24</v>
+      </c>
+      <c r="J1">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>4</v>
+      </c>
+      <c r="O3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E6" s="3"/>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>E2/E3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:I6" si="0">F2/F3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f>M2/M3</f>
+        <v>0.25</v>
+      </c>
+      <c r="O6">
+        <f>N2/N3</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <f>G6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>H2/H3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7" si="1">I2/I3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M7">
+        <f>N6</f>
+        <v>0.25</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>O2/O3</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <f>H6</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G8">
+        <f>H7</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>J2/J3</f>
+        <v>0.5</v>
+      </c>
+      <c r="M8">
+        <f>O6</f>
+        <v>0.5</v>
+      </c>
+      <c r="N8">
+        <f>O7</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f>I6</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>I7</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="H9">
+        <f>I8</f>
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>23</v>
+      </c>
+      <c r="I13">
+        <v>24</v>
+      </c>
+      <c r="J13">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="H14">
+        <v>1.25</v>
+      </c>
+      <c r="I14">
+        <f>0.5+2/3</f>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="J14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>2.5</v>
+      </c>
+      <c r="F15">
+        <v>2.5</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>2.75</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <f>2+2/3</f>
+        <v>2.6666666666666665</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E18" s="3"/>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>E14/E15</f>
+        <v>0.8</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ref="H18" si="2">F14/F15</f>
+        <v>0.4</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ref="I18" si="3">G14/G15</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f>G18</f>
+        <v>0.8</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>H14/H15</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19" si="4">I14/I15</f>
+        <v>0.38888888888888884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <f>H18</f>
+        <v>0.4</v>
+      </c>
+      <c r="G20">
+        <f>H19</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>J14/J15</f>
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <f>I18</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="G21">
+        <f>I19</f>
+        <v>0.38888888888888884</v>
+      </c>
+      <c r="H21">
+        <f>I20</f>
+        <v>0.1875</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="M25" t="s">
+        <v>7</v>
+      </c>
+      <c r="N25" t="s">
+        <v>10</v>
+      </c>
+      <c r="O25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26">
+        <f>1+1/2*2/3</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <f>1+2/3</f>
+        <v>1.6666666666666665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27">
+        <f>2 + 0.5 + (1 - 0.5*1/3)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="N27">
+        <v>4</v>
+      </c>
+      <c r="O27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="M30">
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f>M26/M27</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="O30">
+        <f>N26/N27</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <f>1/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="B31">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M31">
+        <f>N30</f>
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f>O26/O27</f>
+        <v>0.41666666666666663</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <f>O30</f>
+        <v>0.25</v>
+      </c>
+      <c r="N32">
+        <f>O31</f>
+        <v>0.41666666666666663</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:M17"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3165,7 +4421,7 @@
   <dimension ref="A3:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:M17"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6734,573 +7990,2168 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="R1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="6"/>
+      <c r="AF1" s="7"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <f>A3^2</f>
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F6" si="0">B3^2</f>
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G6" si="1">C3^2</f>
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H3">
+        <f>SQRT(SUM(E3:G3))</f>
+        <v>3.7416573867739413</v>
+      </c>
+      <c r="R3" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S3" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T3" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3" t="e">
+        <f>V4</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X3" t="e">
+        <f>V5</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AI3">
+        <f>(A3-B3)^2</f>
+        <v>4</v>
+      </c>
+      <c r="AJ3">
+        <f>(B3-C3)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AK3">
+        <f>(A3-C3)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
+        <f>AM4</f>
+        <v>8.0622577482985491</v>
+      </c>
+      <c r="AO3">
+        <f>AM5</f>
+        <v>4.2426406871192848</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>-1</v>
+      </c>
+      <c r="B4">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E6" si="2">A4^2</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="3">SQRT(SUM(E4:G4))</f>
+        <v>5.0990195135927845</v>
+      </c>
+      <c r="R4" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S4" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T4" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="V4" t="e">
+        <f>R8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4" t="e">
+        <f>W5</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AI4">
+        <f>(A4-B4)^2</f>
+        <v>36</v>
+      </c>
+      <c r="AJ4">
+        <f>(B4-C4)^2</f>
+        <v>25</v>
+      </c>
+      <c r="AK4">
+        <f>(A4-C4)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AM4">
+        <f>AI8</f>
+        <v>8.0622577482985491</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <f>AN5</f>
+        <v>5.196152422706632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="R5" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S5" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T5" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="V5" t="e">
+        <f>T8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="W5" t="e">
+        <f>S8</f>
+        <v>#REF!</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <f>(A5-B5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <f>(B5-C5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <f>(A5-C5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <f>AK8</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="AN5">
+        <f>AJ8</f>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>7.8740078740118111</v>
+      </c>
+      <c r="R6" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S6" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T6" t="e">
+        <f>(#REF!-#REF!)^2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="AI6">
+        <f>(A6-B6)^2</f>
+        <v>25</v>
+      </c>
+      <c r="AJ6">
+        <f>(B6-C6)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AK6">
+        <f>(A6-C6)^2</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="R8" t="e">
+        <f>SQRT(SUM(R3:R6))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="S8" t="e">
+        <f t="shared" ref="S8:T8" si="4">SQRT(SUM(S3:S6))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="T8" t="e">
+        <f t="shared" si="4"/>
+        <v>#REF!</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" ref="AI8:AK8" si="5">SQRT(SUM(AI3:AI6))</f>
+        <v>8.0622577482985491</v>
+      </c>
+      <c r="AJ8">
+        <f t="shared" si="5"/>
+        <v>5.196152422706632</v>
+      </c>
+      <c r="AK8">
+        <f t="shared" si="5"/>
+        <v>4.2426406871192848</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <f>A3*A4</f>
+        <v>-1</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:H9" si="6">B3*B4</f>
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>SUM(F9:H9)</f>
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <f>I9/H3/H4</f>
+        <v>0.73379938570534287</v>
+      </c>
+      <c r="K9">
+        <f>1-COS(J9)</f>
+        <v>0.25736466493128674</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f>K9</f>
+        <v>0.25736466493128674</v>
+      </c>
+      <c r="O9">
+        <f>K13</f>
+        <v>0.3988205586367457</v>
+      </c>
+      <c r="P9">
+        <f>K17</f>
+        <v>0.20084133245389668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <f t="shared" ref="F10:H10" si="7">A4*A5</f>
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:I14" si="8">SUM(F10:H10)</f>
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:J11" si="9">I10/H4/H5</f>
+        <v>0.45291081365783836</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ref="K10:K11" si="10">1-COS(J10)</f>
+        <v>0.10082281414447591</v>
+      </c>
+      <c r="M10">
+        <f>N9</f>
+        <v>0.25736466493128674</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>K10</f>
+        <v>0.10082281414447591</v>
+      </c>
+      <c r="P10">
+        <f>K14</f>
+        <v>2.7902647128695834E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <f t="shared" ref="F11:H11" si="11">A5*A6</f>
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="9"/>
+        <v>0.87988269012811982</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="10"/>
+        <v>0.36275844490660192</v>
+      </c>
+      <c r="M11">
+        <f>O9</f>
+        <v>0.3988205586367457</v>
+      </c>
+      <c r="N11">
+        <f>O10</f>
+        <v>0.10082281414447591</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f>K11</f>
+        <v>0.36275844490660192</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="M12">
+        <f>P9</f>
+        <v>0.20084133245389668</v>
+      </c>
+      <c r="N12">
+        <f>P10</f>
+        <v>2.7902647128695834E-3</v>
+      </c>
+      <c r="O12">
+        <f>P11</f>
+        <v>0.36275844490660192</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f>A3*A5</f>
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:H13" si="12">B3*B5</f>
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="E1">
+      <c r="J13">
+        <f>I13/H3/H5</f>
+        <v>0.92582009977255153</v>
+      </c>
+      <c r="K13">
+        <f>1-COS(J13)</f>
+        <v>0.3988205586367457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <f t="shared" ref="F14:H14" si="13">A4*A6</f>
+        <v>-7</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14" si="14">I14/H4/H6</f>
+        <v>7.4720322208007686E-2</v>
+      </c>
+      <c r="K14">
+        <f>1-COS(J14)</f>
+        <v>2.7902647128695834E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <f>A3*A6</f>
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ref="G17:H17" si="15">B3*B6</f>
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="15"/>
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17" si="16">SUM(F17:H17)</f>
+        <v>19</v>
+      </c>
+      <c r="J17">
+        <f>I17/H3/H6</f>
+        <v>0.64490202163702415</v>
+      </c>
+      <c r="K17">
+        <f>1-COS(J17)</f>
+        <v>0.20084133245389668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <f>A22^2</f>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:F25" si="17">B22^2</f>
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G25" si="18">C22^2</f>
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <f>SQRT(SUM(E22:G22))</f>
+        <v>3.7416573867739413</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>3</v>
+      </c>
+      <c r="T22">
+        <v>2</v>
+      </c>
+      <c r="V22">
+        <f>(R22 - R$26)/SQRT(R$27*2)</f>
+        <v>-0.23570226039551587</v>
+      </c>
+      <c r="W22">
+        <f t="shared" ref="W22:X25" si="19">(S22 - S$26)/SQRT(S$27*2)</f>
+        <v>0.86602540378443871</v>
+      </c>
+      <c r="X22">
+        <f t="shared" si="19"/>
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="Z22">
+        <f>(V22-W22)^2</f>
+        <v>1.2138038460194185</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" ref="AA22:AA25" si="20">(W22-X22)^2</f>
+        <v>0.30227744249483401</v>
+      </c>
+      <c r="AB22">
+        <f>(V22-X22)^2</f>
+        <v>0.30462675405554152</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <f>AD23</f>
+        <v>2</v>
+      </c>
+      <c r="AF22">
+        <f>AD24</f>
+        <v>0.64983939246581257</v>
+      </c>
+      <c r="AI22">
+        <f>(R22-S22)^2</f>
+        <v>4</v>
+      </c>
+      <c r="AJ22">
+        <f t="shared" ref="AJ22:AJ25" si="21">(S22-T22)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AK22">
+        <f>(R22-T22)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AM22">
+        <v>0</v>
+      </c>
+      <c r="AN22">
+        <f>AM23</f>
+        <v>6.2182527020592095</v>
+      </c>
+      <c r="AO22">
+        <f>AM24</f>
+        <v>4.2426406871192848</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>A26^2 + A27</f>
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="17"/>
+        <v>25</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H25" si="22">SQRT(SUM(E23:G23))</f>
+        <v>6.4807406984078604</v>
+      </c>
+      <c r="R23">
+        <v>-1</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <f>(R23 - R$26)/SQRT(R$27*2)</f>
+        <v>-0.70710678118654757</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="19"/>
+        <v>-0.94868329805051377</v>
+      </c>
+      <c r="Z23">
+        <f>V23^2+0.5</f>
+        <v>1</v>
+      </c>
+      <c r="AA23">
+        <f>X23^2+0.5</f>
+        <v>1.4</v>
+      </c>
+      <c r="AB23">
+        <f t="shared" ref="AB23:AB25" si="23">(V23-X23)^2</f>
+        <v>5.8359213500126142E-2</v>
+      </c>
+      <c r="AD23">
+        <f>Z27</f>
+        <v>2</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <f>AE24</f>
+        <v>1.7042754721551525</v>
+      </c>
+      <c r="AI23">
+        <f>(R23-S26)^2+S27</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="AJ23">
+        <f>(S26-T23)^2+S27</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="AK23">
+        <f t="shared" ref="AK23:AK25" si="24">(R23-T23)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AM23">
+        <f>AI27</f>
+        <v>6.2182527020592095</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <f>AN24</f>
+        <v>2.5819888974716112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ref="E23:E25" si="25">A24^2</f>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="22"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="R24">
+        <v>1</v>
+      </c>
+      <c r="S24">
+        <v>1</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="V24">
+        <f>(R24 - R$26)/SQRT(R$27*2)</f>
+        <v>-0.23570226039551587</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="19"/>
+        <v>-0.86602540378443871</v>
+      </c>
+      <c r="X24">
+        <f t="shared" si="19"/>
+        <v>-0.31622776601683794</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" ref="Z24:Z25" si="26">(V24-W24)^2</f>
+        <v>0.39730726509169256</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="20"/>
+        <v>0.30227744249483401</v>
+      </c>
+      <c r="AB24">
+        <f t="shared" si="23"/>
+        <v>6.4843570555695729E-3</v>
+      </c>
+      <c r="AD24">
+        <f>AB27</f>
+        <v>0.64983939246581257</v>
+      </c>
+      <c r="AE24">
+        <f>AA27</f>
+        <v>1.7042754721551525</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <f t="shared" ref="AI24:AI25" si="27">(R24-S24)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AJ24">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AK24">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AM24">
+        <f>AK27</f>
+        <v>4.2426406871192848</v>
+      </c>
+      <c r="AN24">
+        <f>AJ27</f>
+        <v>2.5819888974716112</v>
+      </c>
+      <c r="AO24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="25"/>
+        <v>49</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="18"/>
+        <v>9</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="22"/>
+        <v>7.8740078740118111</v>
+      </c>
+      <c r="R25">
+        <v>7</v>
+      </c>
+      <c r="S25">
+        <v>2</v>
+      </c>
+      <c r="T25">
+        <v>3</v>
+      </c>
+      <c r="V25">
+        <f>(R25 - R$26)/SQRT(R$27*2)</f>
+        <v>1.1785113019775793</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f t="shared" si="19"/>
+        <v>0.94868329805051377</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" si="26"/>
+        <v>1.3888888888888891</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="20"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AB25">
+        <f t="shared" si="23"/>
+        <v>5.282091138909923E-2</v>
+      </c>
+      <c r="AI25">
+        <f t="shared" si="27"/>
+        <v>25</v>
+      </c>
+      <c r="AJ25">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AK25">
+        <f t="shared" si="24"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f>AVERAGE(A22:A25)</f>
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <f t="shared" ref="B26:C26" si="28">AVERAGE(B22:B25)</f>
+        <v>2.75</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="28"/>
+        <v>1.5</v>
+      </c>
+      <c r="R26">
+        <f>AVERAGE(R22:R25)</f>
+        <v>2</v>
+      </c>
+      <c r="S26">
+        <f t="shared" ref="S26:T26" si="29">AVERAGE(S22:S25)</f>
+        <v>2</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="29"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f>_xlfn.VAR.P(A22:A25)</f>
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <f t="shared" ref="B27:C27" si="30">_xlfn.VAR.P(B22:B25)</f>
+        <v>2.1875</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="30"/>
+        <v>1.25</v>
+      </c>
+      <c r="R27">
+        <f>_xlfn.VAR.P(R22:R25)</f>
+        <v>9</v>
+      </c>
+      <c r="S27">
+        <f t="shared" ref="S27:T27" si="31">_xlfn.VAR.P(S22:S25)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="31"/>
+        <v>1.25</v>
+      </c>
+      <c r="Z27">
+        <f>SQRT(SUM(Z22:Z25))</f>
+        <v>2</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" ref="AA27:AB27" si="32">SQRT(SUM(AA22:AA25))</f>
+        <v>1.7042754721551525</v>
+      </c>
+      <c r="AB27">
+        <f t="shared" si="32"/>
+        <v>0.64983939246581257</v>
+      </c>
+      <c r="AI27">
+        <f t="shared" ref="AI27:AK27" si="33">SQRT(SUM(AI22:AI25))</f>
+        <v>6.2182527020592095</v>
+      </c>
+      <c r="AJ27">
+        <f t="shared" si="33"/>
+        <v>2.5819888974716112</v>
+      </c>
+      <c r="AK27">
+        <f t="shared" si="33"/>
+        <v>4.2426406871192848</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <f>A22*A26</f>
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="34">B22*B23</f>
+        <v>15</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ref="H28:H30" si="35">C22*C23</f>
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>SUM(F28:H28)</f>
+        <v>18</v>
+      </c>
+      <c r="J28">
+        <f>I28/H22/H23</f>
+        <v>0.74230748895809029</v>
+      </c>
+      <c r="K28">
+        <f>1-COS(J28)</f>
+        <v>0.26308931778932665</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <f>K28</f>
+        <v>0.26308931778932665</v>
+      </c>
+      <c r="O28">
+        <f>K32</f>
+        <v>0.3988205586367457</v>
+      </c>
+      <c r="P28">
+        <f>K36</f>
+        <v>0.20084133245389668</v>
+      </c>
+    </row>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <f>A26*A24</f>
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="34"/>
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29:I30" si="36">SUM(F29:H29)</f>
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ref="J29:J30" si="37">I29/H23/H24</f>
+        <v>0.71269664509979846</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="K29:K30" si="38">1-COS(J29)</f>
+        <v>0.24339864358583962</v>
+      </c>
+      <c r="M29">
+        <f>N28</f>
+        <v>0.26308931778932665</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f>K29</f>
+        <v>0.24339864358583962</v>
+      </c>
+      <c r="P29">
+        <f>K33</f>
+        <v>0.17891832150255937</v>
+      </c>
+    </row>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <f t="shared" ref="F29:F30" si="39">A24*A25</f>
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="34"/>
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="35"/>
+        <v>3</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="36"/>
         <v>12</v>
       </c>
-      <c r="F1">
-        <v>13</v>
-      </c>
-      <c r="G1">
+      <c r="J30">
+        <f t="shared" si="37"/>
+        <v>0.87988269012811982</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="38"/>
+        <v>0.36275844490660192</v>
+      </c>
+      <c r="M30">
+        <f>O28</f>
+        <v>0.3988205586367457</v>
+      </c>
+      <c r="N30">
+        <f>O29</f>
+        <v>0.24339864358583962</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <f>K30</f>
+        <v>0.36275844490660192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <f>P28</f>
+        <v>0.20084133245389668</v>
+      </c>
+      <c r="N31">
+        <f>P29</f>
+        <v>0.17891832150255937</v>
+      </c>
+      <c r="O31">
+        <f>P30</f>
+        <v>0.36275844490660192</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F32">
+        <f>A22*A24</f>
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ref="G32:G33" si="40">B22*B24</f>
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ref="H32:H33" si="41">C22*C24</f>
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:I33" si="42">SUM(F32:H32)</f>
+        <v>6</v>
+      </c>
+      <c r="J32">
+        <f>I32/H22/H24</f>
+        <v>0.92582009977255153</v>
+      </c>
+      <c r="K32">
+        <f>1-COS(J32)</f>
+        <v>0.3988205586367457</v>
+      </c>
+    </row>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F33">
+        <f>A26*A25</f>
+        <v>21</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="40"/>
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="42"/>
+        <v>31</v>
+      </c>
+      <c r="J33">
+        <f t="shared" ref="J33" si="43">I33/H23/H25</f>
+        <v>0.60749289629395586</v>
+      </c>
+      <c r="K33">
+        <f>1-COS(J33)</f>
+        <v>0.17891832150255937</v>
+      </c>
+    </row>
+    <row r="36" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F36">
+        <f>A22*A25</f>
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <f t="shared" ref="G36" si="44">B22*B25</f>
+        <v>6</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36" si="45">C22*C25</f>
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ref="I36" si="46">SUM(F36:H36)</f>
+        <v>19</v>
+      </c>
+      <c r="J36">
+        <f>I36/H22/H25</f>
+        <v>0.64490202163702415</v>
+      </c>
+      <c r="K36">
+        <f>1-COS(J36)</f>
+        <v>0.20084133245389668</v>
+      </c>
+    </row>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <f>A43^2 + A44</f>
+        <v>25</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ref="F39:F42" si="47">B39^2</f>
+        <v>9</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ref="G39:G42" si="48">C39^2</f>
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <f>SQRT(SUM(E39:G39))</f>
+        <v>6.164414002968976</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+      <c r="S39">
+        <v>3</v>
+      </c>
+      <c r="T39">
+        <v>2</v>
+      </c>
+      <c r="V39">
+        <f>(R39 - R$43)/SQRT(R$44*2)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="W39">
+        <f t="shared" ref="W39:X42" si="49">(S39 - S$43)/SQRT(S$44*2)</f>
+        <v>0.86602540378443871</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="49"/>
+        <v>0.31622776601683794</v>
+      </c>
+      <c r="Z39">
+        <f>(V39-W39)^2</f>
+        <v>1.866025403784439</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" ref="AA39" si="50">(W39-X39)^2</f>
+        <v>0.30227744249483401</v>
+      </c>
+      <c r="AB39">
+        <f>(V39-X39)^2</f>
+        <v>0.66622776601683809</v>
+      </c>
+      <c r="AD39">
+        <v>0</v>
+      </c>
+      <c r="AE39">
+        <f>AD40</f>
+        <v>2</v>
+      </c>
+      <c r="AF39">
+        <f>AD41</f>
+        <v>1.4500460006147986</v>
+      </c>
+      <c r="AI39">
+        <f>(R39-S39)^2</f>
+        <v>4</v>
+      </c>
+      <c r="AJ39">
+        <f t="shared" ref="AJ39" si="51">(S39-T39)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AK39">
+        <f>(R39-T39)^2</f>
+        <v>1</v>
+      </c>
+      <c r="AM39">
+        <v>0</v>
+      </c>
+      <c r="AN39">
+        <f>AM40</f>
+        <v>6.2182527020592095</v>
+      </c>
+      <c r="AO39">
+        <f>AM41</f>
+        <v>5.8309518948453007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <f>A43^2 + A44</f>
+        <v>25</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="47"/>
+        <v>25</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ref="H40:H42" si="52">SQRT(SUM(E40:G40))</f>
+        <v>7.0710678118654755</v>
+      </c>
+      <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="49"/>
+        <v>-0.94868329805051377</v>
+      </c>
+      <c r="Z40">
+        <v>1</v>
+      </c>
+      <c r="AA40">
+        <f>X40^2+0.5</f>
+        <v>1.4</v>
+      </c>
+      <c r="AB40">
+        <f>X40^2+0.5</f>
+        <v>1.4</v>
+      </c>
+      <c r="AD40">
+        <f>Z44</f>
+        <v>2</v>
+      </c>
+      <c r="AE40">
+        <v>0</v>
+      </c>
+      <c r="AF40">
+        <f>AE41</f>
+        <v>1.7042754721551525</v>
+      </c>
+      <c r="AI40">
+        <f>R44+S44+(R43-S43)^2</f>
+        <v>9.6666666666666661</v>
+      </c>
+      <c r="AJ40">
+        <f>(S43-T40)^2+S44</f>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="AK40">
+        <f>(R43-T40)^2+R44</f>
+        <v>17</v>
+      </c>
+      <c r="AM40">
+        <f>AI44</f>
+        <v>6.2182527020592095</v>
+      </c>
+      <c r="AN40">
+        <v>0</v>
+      </c>
+      <c r="AO40">
+        <f>AN41</f>
+        <v>2.5819888974716112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <f t="shared" ref="E41:E43" si="53">A41^2</f>
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="47"/>
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="48"/>
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="52"/>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="V41">
+        <f t="shared" ref="V41:V42" si="54">(R41 - R$43)/SQRT(R$44*2)</f>
+        <v>-0.5</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="49"/>
+        <v>-0.86602540378443871</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="49"/>
+        <v>-0.31622776601683794</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" ref="Z41:AA42" si="55">(V41-W41)^2</f>
+        <v>0.1339745962155614</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="55"/>
+        <v>0.30227744249483401</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" ref="AB41:AB42" si="56">(V41-X41)^2</f>
+        <v>3.3772233983162064E-2</v>
+      </c>
+      <c r="AD41">
+        <f>AB44</f>
+        <v>1.4500460006147986</v>
+      </c>
+      <c r="AE41">
+        <f>AA44</f>
+        <v>1.7042754721551525</v>
+      </c>
+      <c r="AF41">
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <f t="shared" ref="AI41:AJ42" si="57">(R41-S41)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AJ41">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="AK41">
+        <f t="shared" ref="AK41:AK42" si="58">(R41-T41)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AM41">
+        <f>AK44</f>
+        <v>5.8309518948453007</v>
+      </c>
+      <c r="AN41">
+        <f>AJ44</f>
+        <v>2.5819888974716112</v>
+      </c>
+      <c r="AO41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="53"/>
+        <v>49</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="47"/>
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="48"/>
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="52"/>
+        <v>7.8740078740118111</v>
+      </c>
+      <c r="R42">
+        <v>7</v>
+      </c>
+      <c r="S42">
+        <v>2</v>
+      </c>
+      <c r="T42">
+        <v>3</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="49"/>
+        <v>0.94868329805051377</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="55"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="56"/>
+        <v>2.6334038989724042E-3</v>
+      </c>
+      <c r="AI42">
+        <f t="shared" si="57"/>
+        <v>25</v>
+      </c>
+      <c r="AJ42">
+        <f t="shared" si="57"/>
+        <v>1</v>
+      </c>
+      <c r="AK42">
+        <f t="shared" si="58"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f>AVERAGE(A39:A42)</f>
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <f t="shared" ref="B43:C43" si="59">AVERAGE(B39:B42)</f>
+        <v>2.75</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="59"/>
+        <v>1.5</v>
+      </c>
+      <c r="R43">
+        <f>AVERAGE(R39:R42)</f>
+        <v>3</v>
+      </c>
+      <c r="S43">
+        <f t="shared" ref="S43:T43" si="60">AVERAGE(S39:S42)</f>
+        <v>2</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="60"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f>_xlfn.VAR.P(A39:A42)</f>
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <f t="shared" ref="B44:C44" si="61">_xlfn.VAR.P(B39:B42)</f>
+        <v>2.1875</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="61"/>
+        <v>1.25</v>
+      </c>
+      <c r="R44">
+        <f>_xlfn.VAR.P(R39:R42)</f>
+        <v>8</v>
+      </c>
+      <c r="S44">
+        <f t="shared" ref="S44:T44" si="62">_xlfn.VAR.P(S39:S42)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="62"/>
+        <v>1.25</v>
+      </c>
+      <c r="Z44">
+        <f>SQRT(SUM(Z39:Z42))</f>
+        <v>2</v>
+      </c>
+      <c r="AA44">
+        <f t="shared" ref="AA44:AB44" si="63">SQRT(SUM(AA39:AA42))</f>
+        <v>1.7042754721551525</v>
+      </c>
+      <c r="AB44">
+        <f t="shared" si="63"/>
+        <v>1.4500460006147986</v>
+      </c>
+      <c r="AI44">
+        <f t="shared" ref="AI44:AK44" si="64">SQRT(SUM(AI39:AI42))</f>
+        <v>6.2182527020592095</v>
+      </c>
+      <c r="AJ44">
+        <f t="shared" si="64"/>
+        <v>2.5819888974716112</v>
+      </c>
+      <c r="AK44">
+        <f t="shared" si="64"/>
+        <v>5.8309518948453007</v>
+      </c>
+    </row>
+    <row r="45" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F45">
+        <f>A43^2</f>
+        <v>16</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ref="G45:G47" si="65">B39*B40</f>
+        <v>15</v>
+      </c>
+      <c r="H45">
+        <f t="shared" ref="H45:H47" si="66">C39*C40</f>
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f>SUM(F45:H45)</f>
+        <v>31</v>
+      </c>
+      <c r="J45">
+        <f>I45/H39/H40</f>
+        <v>0.71118877499874156</v>
+      </c>
+      <c r="K45">
+        <f>1-COS(J45)</f>
+        <v>0.24241354337043763</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <f>K45</f>
+        <v>0.24241354337043763</v>
+      </c>
+      <c r="O45">
+        <f>K49</f>
+        <v>0.33471977267618036</v>
+      </c>
+      <c r="P45">
+        <f>K53</f>
+        <v>0.32077167953236851</v>
+      </c>
+    </row>
+    <row r="46" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F46">
+        <f>A43*A41</f>
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="65"/>
+        <v>5</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="66"/>
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f t="shared" ref="I46:I47" si="67">SUM(F46:H46)</f>
+        <v>9</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ref="J46:J47" si="68">I46/H40/H41</f>
+        <v>0.73484692283495345</v>
+      </c>
+      <c r="K46">
+        <f t="shared" ref="K46:K47" si="69">1-COS(J46)</f>
+        <v>0.25806660370888956</v>
+      </c>
+      <c r="M46">
+        <f>N45</f>
+        <v>0.24241354337043763</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <f>K46</f>
+        <v>0.25806660370888956</v>
+      </c>
+      <c r="P46">
+        <f>K50</f>
+        <v>0.22400178524578418</v>
+      </c>
+    </row>
+    <row r="47" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="F47">
+        <f t="shared" ref="F47" si="70">A41*A42</f>
+        <v>7</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="65"/>
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="66"/>
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="67"/>
+        <v>12</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="68"/>
+        <v>0.87988269012811982</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="69"/>
+        <v>0.36275844490660192</v>
+      </c>
+      <c r="M47">
+        <f>O45</f>
+        <v>0.33471977267618036</v>
+      </c>
+      <c r="N47">
+        <f>O46</f>
+        <v>0.25806660370888956</v>
+      </c>
+      <c r="O47">
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <f>K47</f>
+        <v>0.36275844490660192</v>
+      </c>
+    </row>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="M48">
+        <f>P45</f>
+        <v>0.32077167953236851</v>
+      </c>
+      <c r="N48">
+        <f>P46</f>
+        <v>0.22400178524578418</v>
+      </c>
+      <c r="O48">
+        <f>P47</f>
+        <v>0.36275844490660192</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F49">
+        <f>A43*A41</f>
+        <v>4</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ref="G49:G50" si="71">B39*B41</f>
+        <v>3</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ref="H49:H50" si="72">C39*C41</f>
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <f t="shared" ref="I49:I50" si="73">SUM(F49:H49)</f>
+        <v>9</v>
+      </c>
+      <c r="J49">
+        <f>I49/H39/H41</f>
+        <v>0.84292723042352469</v>
+      </c>
+      <c r="K49">
+        <f>1-COS(J49)</f>
+        <v>0.33471977267618036</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F50">
+        <f>A43*A42</f>
+        <v>28</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="71"/>
+        <v>10</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="72"/>
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="73"/>
+        <v>38</v>
+      </c>
+      <c r="J50">
+        <f t="shared" ref="J50" si="74">I50/H40/H42</f>
+        <v>0.68250014770174461</v>
+      </c>
+      <c r="K50">
+        <f>1-COS(J50)</f>
+        <v>0.22400178524578418</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11" x14ac:dyDescent="0.2">
+      <c r="F53">
+        <f>A43*A42</f>
+        <v>28</v>
+      </c>
+      <c r="G53">
+        <f t="shared" ref="G53" si="75">B39*B42</f>
+        <v>6</v>
+      </c>
+      <c r="H53">
+        <f t="shared" ref="H53" si="76">C39*C42</f>
+        <v>6</v>
+      </c>
+      <c r="I53">
+        <f t="shared" ref="I53" si="77">SUM(F53:H53)</f>
+        <v>40</v>
+      </c>
+      <c r="J53">
+        <f>I53/H39/H42</f>
+        <v>0.8240856434303292</v>
+      </c>
+      <c r="K53">
+        <f>1-COS(J53)</f>
+        <v>0.32077167953236851</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:N1"/>
+    <mergeCell ref="R1:AF1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:P26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="H1">
-        <v>23</v>
-      </c>
-      <c r="I1">
-        <v>24</v>
-      </c>
-      <c r="J1">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <v>4</v>
-      </c>
-      <c r="N3">
-        <v>4</v>
-      </c>
-      <c r="O3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f>SQRT(2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="F4">
+        <f>1/D4/D5</f>
+        <v>0.49999999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E6" s="3"/>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <f>E2/E3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="H6">
-        <f t="shared" ref="H6:I6" si="0">F2/F3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="I6">
+      <c r="D5">
+        <f>SQRT(2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="F5">
+        <f>1/D3/D5</f>
+        <v>0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>SQRT(1.5)</f>
+        <v>1.2247448713915889</v>
+      </c>
+      <c r="F10">
+        <f>0.5 / D11/D10</f>
+        <v>0.28867513459481287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>SQRT(2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="F11">
+        <f>1/D9/D11</f>
+        <v>0.70710678118654746</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>F23</f>
+        <v>0.63245553203367588</v>
+      </c>
+      <c r="K19">
+        <f>F26</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="M19">
+        <f>1-COS(H19)</f>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ref="N19:N22" si="0">1-COS(I19)</f>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19:O22" si="1">1-COS(J19)</f>
+        <v>0.19342159011492444</v>
+      </c>
+      <c r="P19">
+        <f t="shared" ref="P19:P22" si="2">1-COS(K19)</f>
+        <v>0.16208817230500694</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>SQRT(1.5)</f>
+        <v>1.2247448713915889</v>
+      </c>
+      <c r="F20">
+        <f>1.5/D20/D21</f>
+        <v>0.7745966692414834</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>F20</f>
+        <v>0.7745966692414834</v>
+      </c>
+      <c r="K20">
+        <f>F24</f>
+        <v>0.70710678118654768</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ref="M20:M22" si="3">1-COS(H20)</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <f>M2/M3</f>
-        <v>0.25</v>
-      </c>
-      <c r="O6">
-        <f>N2/N3</f>
+      <c r="O20">
+        <f t="shared" si="1"/>
+        <v>0.28529680704577487</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>0.23975540292436992</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <f>SQRT(2.5)</f>
+        <v>1.5811388300841898</v>
+      </c>
+      <c r="F21">
+        <f>2.5/D21/D22</f>
+        <v>0.91287092917527679</v>
+      </c>
+      <c r="H21">
+        <f>J19</f>
+        <v>0.63245553203367588</v>
+      </c>
+      <c r="I21">
+        <f>J20</f>
+        <v>0.7745966692414834</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>F21</f>
+        <v>0.91287092917527679</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>0.19342159011492444</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="0"/>
+        <v>0.28529680704577487</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>0.38852338603420733</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f>SQRT(3)</f>
+        <v>1.7320508075688772</v>
+      </c>
+      <c r="H22">
+        <f>K19</f>
+        <v>0.57735026918962584</v>
+      </c>
+      <c r="I22">
+        <f>K20</f>
+        <v>0.70710678118654768</v>
+      </c>
+      <c r="J22">
+        <f>K21</f>
+        <v>0.91287092917527679</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="3"/>
+        <v>0.16208817230500694</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="0"/>
+        <v>0.23975540292436992</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="1"/>
+        <v>0.38852338603420733</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0.75</v>
+      </c>
+      <c r="B23">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F7">
-        <f>G6</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f>H2/H3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ref="I7" si="1">I2/I3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="M7">
-        <f>N6</f>
-        <v>0.25</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <f>O2/O3</f>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F8">
-        <f>H6</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G8">
-        <f>H7</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f>J2/J3</f>
-        <v>0.5</v>
-      </c>
-      <c r="M8">
-        <f>O6</f>
-        <v>0.5</v>
-      </c>
-      <c r="N8">
-        <f>O7</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F9">
-        <f>I6</f>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <f>I7</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="H9">
-        <f>I8</f>
-        <v>0.5</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>14</v>
-      </c>
-      <c r="H13">
-        <v>23</v>
-      </c>
-      <c r="I13">
-        <v>24</v>
-      </c>
-      <c r="J13">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="H14">
-        <v>1.25</v>
-      </c>
-      <c r="I14">
-        <f>0.5+2/3</f>
-        <v>1.1666666666666665</v>
-      </c>
-      <c r="J14">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>2.5</v>
-      </c>
-      <c r="F15">
-        <v>2.5</v>
-      </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>2.75</v>
-      </c>
-      <c r="I15">
-        <v>3</v>
-      </c>
-      <c r="J15">
-        <f>2+2/3</f>
-        <v>2.6666666666666665</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E18" s="3"/>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f>E14/E15</f>
-        <v>0.8</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ref="H18" si="2">F14/F15</f>
-        <v>0.4</v>
-      </c>
-      <c r="I18">
-        <f t="shared" ref="I18" si="3">G14/G15</f>
-        <v>0.22222222222222221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F19">
-        <f>G18</f>
-        <v>0.8</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <f>H14/H15</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="I19">
-        <f t="shared" ref="I19" si="4">I14/I15</f>
-        <v>0.38888888888888884</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F20">
-        <f>H18</f>
-        <v>0.4</v>
-      </c>
-      <c r="G20">
-        <f>H19</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f>J14/J15</f>
-        <v>0.1875</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="F21">
-        <f>I18</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="G21">
-        <f>I19</f>
-        <v>0.38888888888888884</v>
-      </c>
-      <c r="H21">
-        <f>I20</f>
-        <v>0.1875</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="M25" t="s">
-        <v>7</v>
-      </c>
-      <c r="N25" t="s">
-        <v>10</v>
-      </c>
-      <c r="O25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26">
-        <f>1+1/2*2/3</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26">
-        <f>1+2/3</f>
-        <v>1.6666666666666665</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27">
-        <f>2 + 0.5 + (1 - 0.5*1/3)</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="N27">
-        <v>4</v>
-      </c>
-      <c r="O27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="M30">
-        <v>0</v>
-      </c>
-      <c r="N30">
-        <f>M26/M27</f>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="O30">
-        <f>N26/N27</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
-        <f>1/2</f>
-        <v>0.5</v>
-      </c>
-      <c r="B31">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="M31">
-        <f>N30</f>
-        <v>0.39999999999999997</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <f>O26/O27</f>
-        <v>0.41666666666666663</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M32">
-        <f>O30</f>
-        <v>0.25</v>
-      </c>
-      <c r="N32">
-        <f>O31</f>
-        <v>0.41666666666666663</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
+      <c r="C23">
+        <v>0.75</v>
+      </c>
+      <c r="F23">
+        <f>1/D19/D21</f>
+        <v>0.63245553203367588</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <f>1.5/D20/D22</f>
+        <v>0.70710678118654768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <f>1/D19/D22</f>
+        <v>0.57735026918962584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
distances: Speed up all distances
</commit_message>
<xml_diff>
--- a/Orange/distance/tests/calculation.xlsx
+++ b/Orange/distance/tests/calculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="disc - eucl+manh" sheetId="2" r:id="rId1"/>
@@ -168,8 +168,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="157">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -348,7 +362,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="157">
+  <cellStyles count="171">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -427,6 +441,13 @@
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -505,6 +526,13 @@
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1184,7 +1212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1464,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="K27">
-        <f t="shared" ref="J27:L27" si="14">B$23*B3</f>
+        <f t="shared" ref="K27:L27" si="14">B$23*B3</f>
         <v>6</v>
       </c>
       <c r="L27">
@@ -1486,7 +1514,7 @@
         <v>9</v>
       </c>
       <c r="K28">
-        <f t="shared" ref="J28:L28" si="15">B$23*B4</f>
+        <f t="shared" ref="K28:L28" si="15">B$23*B4</f>
         <v>10</v>
       </c>
       <c r="L28">
@@ -1508,7 +1536,7 @@
         <v>3</v>
       </c>
       <c r="K29">
-        <f t="shared" ref="J29:L29" si="19">B$23*B5</f>
+        <f t="shared" ref="K29:L29" si="19">B$23*B5</f>
         <v>2</v>
       </c>
       <c r="L29">
@@ -1530,7 +1558,7 @@
         <v>21</v>
       </c>
       <c r="K30">
-        <f t="shared" ref="J30:L30" si="20">B$23*B6</f>
+        <f t="shared" ref="K30:L30" si="20">B$23*B6</f>
         <v>4</v>
       </c>
       <c r="L30">
@@ -1574,7 +1602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -8078,7 +8106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO53"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="P48" sqref="M45:P48"/>
     </sheetView>
   </sheetViews>
@@ -8661,7 +8689,7 @@
       </c>
       <c r="AE22">
         <f>Z26/Z29/AA29</f>
-        <v>0.51355259101309547</v>
+        <v>0.52297636036849082</v>
       </c>
       <c r="AF22">
         <f>AB26/Z29/AB29</f>
@@ -8673,7 +8701,7 @@
       </c>
       <c r="AI22">
         <f t="shared" ref="AI22:AI24" si="30">1-AE22</f>
-        <v>0.48644740898690453</v>
+        <v>0.47702363963150918</v>
       </c>
       <c r="AJ22">
         <f t="shared" ref="AJ22:AJ24" si="31">1-AF22</f>
@@ -8688,8 +8716,8 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <f>A26^2 + A27</f>
-        <v>17</v>
+        <f>A26^2</f>
+        <v>9</v>
       </c>
       <c r="F23">
         <f t="shared" si="25"/>
@@ -8701,7 +8729,7 @@
       </c>
       <c r="H23">
         <f t="shared" ref="H23:H25" si="32">SQRT(SUM(E23:G23))</f>
-        <v>6.4807406984078604</v>
+        <v>5.8309518948453007</v>
       </c>
       <c r="R23">
         <v>-1</v>
@@ -8714,8 +8742,8 @@
         <v>1</v>
       </c>
       <c r="W23">
-        <f>S26^2+S27</f>
-        <v>4.666666666666667</v>
+        <f>S26^2</f>
+        <v>4</v>
       </c>
       <c r="X23">
         <f t="shared" si="28"/>
@@ -8735,18 +8763,18 @@
       </c>
       <c r="AD23">
         <f>AE22</f>
-        <v>0.51355259101309547</v>
+        <v>0.52297636036849082</v>
       </c>
       <c r="AE23">
         <v>1</v>
       </c>
       <c r="AF23">
         <f>AA26/AA29/AB29</f>
-        <v>0.80416644637126444</v>
+        <v>0.8189230248533258</v>
       </c>
       <c r="AH23">
         <f t="shared" ref="AH23:AH24" si="34">1-AD23</f>
-        <v>0.48644740898690453</v>
+        <v>0.47702363963150918</v>
       </c>
       <c r="AI23">
         <f t="shared" si="30"/>
@@ -8754,7 +8782,7 @@
       </c>
       <c r="AJ23">
         <f t="shared" si="31"/>
-        <v>0.19583355362873556</v>
+        <v>0.1810769751466742</v>
       </c>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.2">
@@ -8822,7 +8850,7 @@
       </c>
       <c r="AE24">
         <f>AF23</f>
-        <v>0.80416644637126444</v>
+        <v>0.8189230248533258</v>
       </c>
       <c r="AF24">
         <v>1</v>
@@ -8833,7 +8861,7 @@
       </c>
       <c r="AI24">
         <f t="shared" si="30"/>
-        <v>0.19583355362873556</v>
+        <v>0.1810769751466742</v>
       </c>
       <c r="AJ24">
         <f t="shared" si="31"/>
@@ -8983,18 +9011,18 @@
       </c>
       <c r="J28">
         <f>I28/H22/H23</f>
-        <v>0.74230748895809029</v>
+        <v>0.82502864732539016</v>
       </c>
       <c r="K28">
         <f t="shared" ref="K28:K30" si="46">1-J28</f>
-        <v>0.25769251104190971</v>
+        <v>0.17497135267460984</v>
       </c>
       <c r="M28">
         <v>0</v>
       </c>
       <c r="N28">
         <f>K28</f>
-        <v>0.25769251104190971</v>
+        <v>0.17497135267460984</v>
       </c>
       <c r="O28">
         <f>K32</f>
@@ -9010,7 +9038,7 @@
       </c>
       <c r="AA28">
         <f t="shared" ref="AA28:AB28" si="47">SUM(W22:W25)</f>
-        <v>18.666666666666668</v>
+        <v>18</v>
       </c>
       <c r="AB28">
         <f t="shared" si="47"/>
@@ -9036,26 +9064,26 @@
       </c>
       <c r="J29">
         <f t="shared" ref="J29:J30" si="49">I29/H23/H24</f>
-        <v>0.71269664509979846</v>
+        <v>0.79211803438133943</v>
       </c>
       <c r="K29">
         <f t="shared" si="46"/>
-        <v>0.28730335490020154</v>
+        <v>0.20788196561866057</v>
       </c>
       <c r="M29">
         <f>N28</f>
-        <v>0.25769251104190971</v>
+        <v>0.17497135267460984</v>
       </c>
       <c r="N29">
         <v>0</v>
       </c>
       <c r="O29">
         <f>K29</f>
-        <v>0.28730335490020154</v>
+        <v>0.20788196561866057</v>
       </c>
       <c r="P29">
         <f>K33</f>
-        <v>0.39250710370604414</v>
+        <v>0.32480939510300022</v>
       </c>
       <c r="Z29">
         <f>SQRT(Z28)</f>
@@ -9063,7 +9091,7 @@
       </c>
       <c r="AA29">
         <f t="shared" ref="AA29" si="50">SQRT(AA28)</f>
-        <v>4.3204937989385739</v>
+        <v>4.2426406871192848</v>
       </c>
       <c r="AB29">
         <f t="shared" ref="AB29" si="51">SQRT(AB28)</f>
@@ -9101,7 +9129,7 @@
       </c>
       <c r="N30">
         <f>O29</f>
-        <v>0.28730335490020154</v>
+        <v>0.20788196561866057</v>
       </c>
       <c r="O30">
         <v>0</v>
@@ -9118,7 +9146,7 @@
       </c>
       <c r="N31">
         <f>P29</f>
-        <v>0.39250710370604414</v>
+        <v>0.32480939510300022</v>
       </c>
       <c r="O31">
         <f>P30</f>
@@ -9173,11 +9201,11 @@
       </c>
       <c r="J33">
         <f t="shared" ref="J33" si="57">I33/H23/H25</f>
-        <v>0.60749289629395586</v>
+        <v>0.67519060489699978</v>
       </c>
       <c r="K33">
         <f t="shared" si="56"/>
-        <v>0.39250710370604414</v>
+        <v>0.32480939510300022</v>
       </c>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.2">
@@ -9214,8 +9242,8 @@
         <v>2</v>
       </c>
       <c r="E39">
-        <f>A43^2 + A44</f>
-        <v>25</v>
+        <f>A43^2</f>
+        <v>16</v>
       </c>
       <c r="F39">
         <f t="shared" ref="F39:F42" si="61">B39^2</f>
@@ -9227,7 +9255,7 @@
       </c>
       <c r="H39">
         <f>SQRT(SUM(E39:G39))</f>
-        <v>6.164414002968976</v>
+        <v>5.3851648071345037</v>
       </c>
       <c r="R39">
         <v>1</v>
@@ -9243,7 +9271,7 @@
         <v>1</v>
       </c>
       <c r="W39">
-        <f t="shared" ref="W39:W42" si="63">S39^2</f>
+        <f t="shared" ref="W39" si="63">S39^2</f>
         <v>9</v>
       </c>
       <c r="X39">
@@ -9255,7 +9283,7 @@
         <v>3</v>
       </c>
       <c r="AA39">
-        <f t="shared" ref="AA39:AA42" si="65">S39*T39</f>
+        <f t="shared" ref="AA39" si="65">S39*T39</f>
         <v>6</v>
       </c>
       <c r="AB39">
@@ -9267,11 +9295,11 @@
       </c>
       <c r="AE39">
         <f>Z43/Z46/AA46</f>
-        <v>0.6736330697086077</v>
+        <v>0.73029674334022154</v>
       </c>
       <c r="AF39">
         <f>AB43/Z46/AB46</f>
-        <v>0.85749292571254421</v>
+        <v>0.9128709291752769</v>
       </c>
       <c r="AH39">
         <f>1-AD39</f>
@@ -9279,11 +9307,11 @@
       </c>
       <c r="AI39">
         <f t="shared" ref="AI39:AI41" si="66">1-AE39</f>
-        <v>0.3263669302913923</v>
+        <v>0.26970325665977846</v>
       </c>
       <c r="AJ39">
         <f t="shared" ref="AJ39:AJ41" si="67">1-AF39</f>
-        <v>0.14250707428745579</v>
+        <v>8.7129070824723098E-2</v>
       </c>
       <c r="AM39">
         <v>0</v>
@@ -9305,8 +9333,8 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <f>A43^2 + A44</f>
-        <v>25</v>
+        <f>A43^2</f>
+        <v>16</v>
       </c>
       <c r="F40">
         <f t="shared" si="61"/>
@@ -9318,18 +9346,18 @@
       </c>
       <c r="H40">
         <f t="shared" ref="H40:H42" si="68">SQRT(SUM(E40:G40))</f>
-        <v>7.0710678118654755</v>
+        <v>6.4031242374328485</v>
       </c>
       <c r="T40">
         <v>2</v>
       </c>
       <c r="V40">
-        <f>R43^2+R44</f>
-        <v>17</v>
+        <f>R43^2</f>
+        <v>9</v>
       </c>
       <c r="W40">
-        <f>S43^2+S44</f>
-        <v>4.666666666666667</v>
+        <f>S43^2</f>
+        <v>4</v>
       </c>
       <c r="X40">
         <f t="shared" si="64"/>
@@ -9349,18 +9377,18 @@
       </c>
       <c r="AD40">
         <f>AE39</f>
-        <v>0.6736330697086077</v>
+        <v>0.73029674334022154</v>
       </c>
       <c r="AE40">
         <v>1</v>
       </c>
       <c r="AF40">
         <f>AA43/AA46/AB46</f>
-        <v>0.9274260335029676</v>
+        <v>0.94444444444444464</v>
       </c>
       <c r="AH40">
         <f t="shared" ref="AH40:AH41" si="69">1-AD40</f>
-        <v>0.3263669302913923</v>
+        <v>0.26970325665977846</v>
       </c>
       <c r="AI40">
         <f t="shared" si="66"/>
@@ -9368,7 +9396,7 @@
       </c>
       <c r="AJ40">
         <f t="shared" si="67"/>
-        <v>7.2573966497032405E-2</v>
+        <v>5.5555555555555358E-2</v>
       </c>
       <c r="AM40">
         <f>AI44</f>
@@ -9418,11 +9446,11 @@
         <v>1</v>
       </c>
       <c r="V41">
-        <f t="shared" ref="V40:V42" si="71">R41^2</f>
+        <f t="shared" ref="V41:V42" si="71">R41^2</f>
         <v>1</v>
       </c>
       <c r="W41">
-        <f t="shared" ref="W41:W44" si="72">S41^2</f>
+        <f t="shared" ref="W41:W42" si="72">S41^2</f>
         <v>1</v>
       </c>
       <c r="X41">
@@ -9434,7 +9462,7 @@
         <v>1</v>
       </c>
       <c r="AA41">
-        <f t="shared" ref="AA41:AA44" si="74">S41*T41</f>
+        <f t="shared" ref="AA41:AA42" si="74">S41*T41</f>
         <v>1</v>
       </c>
       <c r="AB41">
@@ -9443,22 +9471,22 @@
       </c>
       <c r="AD41">
         <f>AF39</f>
-        <v>0.85749292571254421</v>
+        <v>0.9128709291752769</v>
       </c>
       <c r="AE41">
         <f>AF40</f>
-        <v>0.9274260335029676</v>
+        <v>0.94444444444444464</v>
       </c>
       <c r="AF41">
         <v>1</v>
       </c>
       <c r="AH41">
         <f t="shared" si="69"/>
-        <v>0.14250707428745579</v>
+        <v>8.7129070824723098E-2</v>
       </c>
       <c r="AI41">
         <f t="shared" si="66"/>
-        <v>7.2573966497032405E-2</v>
+        <v>5.5555555555555358E-2</v>
       </c>
       <c r="AJ41">
         <f t="shared" si="67"/>
@@ -9619,34 +9647,34 @@
       </c>
       <c r="J45">
         <f>I45/H39/H40</f>
-        <v>0.71118877499874156</v>
+        <v>0.89902292537689943</v>
       </c>
       <c r="K45">
         <f t="shared" ref="K45:K47" si="84">1-J45</f>
-        <v>0.28881122500125844</v>
+        <v>0.10097707462310057</v>
       </c>
       <c r="M45">
         <v>0</v>
       </c>
       <c r="N45">
         <f>K45</f>
-        <v>0.28881122500125844</v>
+        <v>0.10097707462310057</v>
       </c>
       <c r="O45">
         <f>K49</f>
-        <v>0.15707276957647531</v>
+        <v>3.5098718645984461E-2</v>
       </c>
       <c r="P45">
         <f>K53</f>
-        <v>0.1759143565696708</v>
+        <v>5.6666738726843469E-2</v>
       </c>
       <c r="Z45">
         <f>SUM(V39:V42)</f>
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="AA45">
         <f t="shared" ref="AA45" si="85">SUM(W39:W42)</f>
-        <v>18.666666666666668</v>
+        <v>18</v>
       </c>
       <c r="AB45">
         <f t="shared" ref="AB45" si="86">SUM(X39:X42)</f>
@@ -9672,34 +9700,34 @@
       </c>
       <c r="J46">
         <f t="shared" ref="J46:J47" si="88">I46/H40/H41</f>
-        <v>0.73484692283495345</v>
+        <v>0.8115026712006892</v>
       </c>
       <c r="K46">
         <f t="shared" si="84"/>
-        <v>0.26515307716504655</v>
+        <v>0.1884973287993108</v>
       </c>
       <c r="M46">
         <f>N45</f>
-        <v>0.28881122500125844</v>
+        <v>0.10097707462310057</v>
       </c>
       <c r="N46">
         <v>0</v>
       </c>
       <c r="O46">
         <f>K46</f>
-        <v>0.26515307716504655</v>
+        <v>0.1884973287993108</v>
       </c>
       <c r="P46">
         <f>K50</f>
-        <v>0.31749985229825539</v>
+        <v>0.24630467142988177</v>
       </c>
       <c r="Z46">
         <f>SQRT(Z45)</f>
-        <v>8.2462112512353212</v>
+        <v>7.745966692414834</v>
       </c>
       <c r="AA46">
         <f t="shared" ref="AA46" si="89">SQRT(AA45)</f>
-        <v>4.3204937989385739</v>
+        <v>4.2426406871192848</v>
       </c>
       <c r="AB46">
         <f t="shared" ref="AB46" si="90">SQRT(AB45)</f>
@@ -9733,11 +9761,11 @@
       </c>
       <c r="M47">
         <f>O45</f>
-        <v>0.15707276957647531</v>
+        <v>3.5098718645984461E-2</v>
       </c>
       <c r="N47">
         <f>O46</f>
-        <v>0.26515307716504655</v>
+        <v>0.1884973287993108</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -9750,11 +9778,11 @@
     <row r="48" spans="1:41" x14ac:dyDescent="0.2">
       <c r="M48">
         <f>P45</f>
-        <v>0.1759143565696708</v>
+        <v>5.6666738726843469E-2</v>
       </c>
       <c r="N48">
         <f>P46</f>
-        <v>0.31749985229825539</v>
+        <v>0.24630467142988177</v>
       </c>
       <c r="O48">
         <f>P47</f>
@@ -9783,11 +9811,11 @@
       </c>
       <c r="J49">
         <f>I49/H39/H41</f>
-        <v>0.84292723042352469</v>
+        <v>0.96490128135401554</v>
       </c>
       <c r="K49">
         <f t="shared" ref="K49:K50" si="95">1-J49</f>
-        <v>0.15707276957647531</v>
+        <v>3.5098718645984461E-2</v>
       </c>
     </row>
     <row r="50" spans="6:11" x14ac:dyDescent="0.2">
@@ -9809,11 +9837,11 @@
       </c>
       <c r="J50">
         <f t="shared" ref="J50" si="96">I50/H40/H42</f>
-        <v>0.68250014770174461</v>
+        <v>0.75369532857011823</v>
       </c>
       <c r="K50">
         <f t="shared" si="95"/>
-        <v>0.31749985229825539</v>
+        <v>0.24630467142988177</v>
       </c>
     </row>
     <row r="53" spans="6:11" x14ac:dyDescent="0.2">
@@ -9835,11 +9863,11 @@
       </c>
       <c r="J53">
         <f>I53/H39/H42</f>
-        <v>0.8240856434303292</v>
+        <v>0.94333326127315653</v>
       </c>
       <c r="K53">
         <f>1-J53</f>
-        <v>0.1759143565696708</v>
+        <v>5.6666738726843469E-2</v>
       </c>
     </row>
   </sheetData>
@@ -9857,7 +9885,7 @@
   <dimension ref="A2:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="M19:P22"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9947,12 +9975,12 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <f>SQRT(1.5)</f>
-        <v>1.2247448713915889</v>
+        <f>SQRT(1.25)</f>
+        <v>1.1180339887498949</v>
       </c>
       <c r="F10">
         <f>0.5 / D11/D10</f>
-        <v>0.28867513459481287</v>
+        <v>0.31622776601683789</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -9998,7 +10026,7 @@
       </c>
       <c r="J19">
         <f>F23</f>
-        <v>0.63245553203367588</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="K19">
         <f>F26</f>
@@ -10013,10 +10041,10 @@
       </c>
       <c r="O19">
         <f t="shared" ref="O19:O22" si="1">1-J19</f>
-        <v>0.36754446796632412</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19:P22" si="2">1-K19</f>
+        <f t="shared" ref="P19:P21" si="2">1-K19</f>
         <v>0.42264973081037416</v>
       </c>
     </row>
@@ -10028,12 +10056,12 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <f>SQRT(1.5)</f>
-        <v>1.2247448713915889</v>
+        <f>SQRT(1.25)</f>
+        <v>1.1180339887498949</v>
       </c>
       <c r="F20">
-        <f>1.5/D20/D21</f>
-        <v>0.7745966692414834</v>
+        <f>1.25/D20/D21</f>
+        <v>0.7453559924999299</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -10043,11 +10071,11 @@
       </c>
       <c r="J20">
         <f>F20</f>
-        <v>0.7745966692414834</v>
+        <v>0.7453559924999299</v>
       </c>
       <c r="K20">
         <f>F24</f>
-        <v>0.70710678118654768</v>
+        <v>0.7745966692414834</v>
       </c>
       <c r="M20">
         <f t="shared" ref="M20:M22" si="3">1-H20</f>
@@ -10058,11 +10086,11 @@
       </c>
       <c r="O20">
         <f t="shared" si="1"/>
-        <v>0.2254033307585166</v>
+        <v>0.2546440075000701</v>
       </c>
       <c r="P20">
         <f t="shared" si="2"/>
-        <v>0.29289321881345232</v>
+        <v>0.2254033307585166</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
@@ -10073,42 +10101,42 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <f>SQRT(2.5)</f>
-        <v>1.5811388300841898</v>
+        <f>SQRT(2.25)</f>
+        <v>1.5</v>
       </c>
       <c r="F21">
         <f>2.5/D21/D22</f>
-        <v>0.91287092917527679</v>
+        <v>0.96225044864937637</v>
       </c>
       <c r="H21">
         <f>J19</f>
-        <v>0.63245553203367588</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I21">
         <f>J20</f>
-        <v>0.7745966692414834</v>
+        <v>0.7453559924999299</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
         <f>F21</f>
-        <v>0.91287092917527679</v>
+        <v>0.96225044864937637</v>
       </c>
       <c r="M21">
         <f t="shared" si="3"/>
-        <v>0.36754446796632412</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="N21">
         <f t="shared" si="0"/>
-        <v>0.2254033307585166</v>
+        <v>0.2546440075000701</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21">
         <f t="shared" si="2"/>
-        <v>8.7129070824723209E-2</v>
+        <v>3.7749551350623634E-2</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
@@ -10131,11 +10159,11 @@
       </c>
       <c r="I22">
         <f>K20</f>
-        <v>0.70710678118654768</v>
+        <v>0.7745966692414834</v>
       </c>
       <c r="J22">
         <f>K21</f>
-        <v>0.91287092917527679</v>
+        <v>0.96225044864937637</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -10146,11 +10174,11 @@
       </c>
       <c r="N22">
         <f t="shared" si="0"/>
-        <v>0.29289321881345232</v>
+        <v>0.2254033307585166</v>
       </c>
       <c r="O22">
         <f t="shared" si="1"/>
-        <v>8.7129070824723209E-2</v>
+        <v>3.7749551350623634E-2</v>
       </c>
       <c r="P22">
         <v>0</v>
@@ -10168,13 +10196,13 @@
       </c>
       <c r="F23">
         <f>1/D19/D21</f>
-        <v>0.63245553203367588</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="F24">
         <f>1.5/D20/D22</f>
-        <v>0.70710678118654768</v>
+        <v>0.7745966692414834</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>